<commit_message>
Excel modified added heading
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Demo\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39E58CF8-16E5-4AEB-B95E-64185F09EF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E661694F-4557-4635-B4D6-0213853B341E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2F07E8C1-4BDC-414A-9E04-C0CF2B6BCF13}"/>
   </bookViews>
@@ -35,10 +35,26 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Heading</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,269 +399,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CD84FC-033D-4ACB-981E-D6BBE249056D}">
-  <dimension ref="A1:A52"/>
+  <dimension ref="A1:A53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>64833</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>64834</v>
+        <v>64833</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>64835</v>
+        <v>64834</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>64836</v>
+        <v>64835</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>64837</v>
+        <v>64836</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>64838</v>
+        <v>64837</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>64839</v>
+        <v>64838</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>64840</v>
+        <v>64839</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>64841</v>
+        <v>64840</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>64842</v>
+        <v>64841</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>64843</v>
+        <v>64842</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>64844</v>
+        <v>64843</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>64845</v>
+        <v>64844</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>64846</v>
+        <v>64845</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>64847</v>
+        <v>64846</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>64848</v>
+        <v>64847</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>64849</v>
+        <v>64848</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>64850</v>
+        <v>64849</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>64851</v>
+        <v>64850</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>64852</v>
+        <v>64851</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>64853</v>
+        <v>64852</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>64854</v>
+        <v>64853</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>64855</v>
+        <v>64854</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>64856</v>
+        <v>64855</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>64857</v>
+        <v>64856</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>64858</v>
+        <v>64857</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>64859</v>
+        <v>64858</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>64860</v>
+        <v>64859</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>64861</v>
+        <v>64860</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>64862</v>
+        <v>64861</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>64863</v>
+        <v>64862</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>64864</v>
+        <v>64863</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>64865</v>
+        <v>64864</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>64866</v>
+        <v>64865</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>64867</v>
+        <v>64866</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>64868</v>
+        <v>64867</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>64869</v>
+        <v>64868</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>64870</v>
+        <v>64869</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>64871</v>
+        <v>64870</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>64872</v>
+        <v>64871</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>64873</v>
+        <v>64872</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>64874</v>
+        <v>64873</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>64875</v>
+        <v>64874</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>64876</v>
+        <v>64875</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>64877</v>
+        <v>64876</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>64878</v>
+        <v>64877</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>64879</v>
+        <v>64878</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>64880</v>
+        <v>64879</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>64881</v>
+        <v>64880</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>64882</v>
+        <v>64881</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>64883</v>
+        <v>64882</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52">
+        <v>64883</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53">
         <v>64884</v>
       </c>
     </row>

</xml_diff>